<commit_message>
fix curitiba after changing time dimensions in Emissions
</commit_message>
<xml_diff>
--- a/projects/brazil_bu_csv/config/inventory.xlsx
+++ b/projects/brazil_bu_csv/config/inventory.xlsx
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -309,7 +309,7 @@
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.48"/>
@@ -755,7 +755,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -764,7 +764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -774,7 +774,7 @@
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4183,7 +4183,7 @@
   <autoFilter ref="A1:AA41"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4193,7 +4193,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4203,7 +4203,7 @@
       <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="17.67"/>
@@ -6326,7 +6326,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -6335,7 +6335,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6345,7 +6345,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="8.67"/>
@@ -9776,7 +9776,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -9785,7 +9785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -9795,7 +9795,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.43"/>
@@ -9849,7 +9849,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -9858,17 +9858,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -9886,98 +9886,10 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>22.8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>20.3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>16.9</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>16.2</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>18.3</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>19.2</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>20.2</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>22.5</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>